<commit_message>
avances en el informe del nshore y added doc con estructura de informe de tesis
</commit_message>
<xml_diff>
--- a/neuralito/ArfGen/docs/Entregas/5ta entrega - Evaluaciones/North Shore/NoBuoyStrategy[2003,2004]/North shore.xlsx
+++ b/neuralito/ArfGen/docs/Entregas/5ta entrega - Evaluaciones/North Shore/NoBuoyStrategy[2003,2004]/North shore.xlsx
@@ -589,25 +589,25 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="63237504"/>
-        <c:axId val="63317120"/>
+        <c:axId val="63106432"/>
+        <c:axId val="63513728"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="63237504"/>
+        <c:axId val="63106432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="63317120"/>
+        <c:crossAx val="63513728"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="63317120"/>
+        <c:axId val="63513728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -621,7 +621,7 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="63237504"/>
+        <c:crossAx val="63106432"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -634,7 +634,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
+    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1053,11 +1053,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="64381312"/>
-        <c:axId val="64383232"/>
+        <c:axId val="64315776"/>
+        <c:axId val="64317696"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="64381312"/>
+        <c:axId val="64315776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1084,12 +1084,12 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="64383232"/>
+        <c:crossAx val="64317696"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="64383232"/>
+        <c:axId val="64317696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1116,7 +1116,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="64381312"/>
+        <c:crossAx val="64315776"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1125,7 +1125,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
+    <c:pageMargins b="0.75000000000000056" l="0.70000000000000051" r="0.70000000000000051" t="0.75000000000000056" header="0.30000000000000027" footer="0.30000000000000027"/>
     <c:pageSetup/>
   </c:printSettings>
   <c:userShapes r:id="rId1"/>
@@ -1152,7 +1152,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
     </c:title>
     <c:plotArea>
       <c:layout/>
@@ -5019,25 +5018,25 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="64436864"/>
-        <c:axId val="64442752"/>
+        <c:axId val="64363136"/>
+        <c:axId val="64369024"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="64436864"/>
+        <c:axId val="64363136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="64442752"/>
+        <c:crossAx val="64369024"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="64442752"/>
+        <c:axId val="64369024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5051,20 +5050,19 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="64436864"/>
+        <c:crossAx val="64363136"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
+    <c:pageMargins b="0.75000000000000056" l="0.70000000000000051" r="0.70000000000000051" t="0.75000000000000056" header="0.30000000000000027" footer="0.30000000000000027"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -8933,11 +8931,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="64479232"/>
-        <c:axId val="64481152"/>
+        <c:axId val="64409600"/>
+        <c:axId val="64411520"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="64479232"/>
+        <c:axId val="64409600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8960,16 +8958,15 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="64481152"/>
+        <c:crossAx val="64411520"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="64481152"/>
+        <c:axId val="64411520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8992,11 +8989,10 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="64479232"/>
+        <c:crossAx val="64409600"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -9005,7 +9001,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
+    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
     <c:pageSetup/>
   </c:printSettings>
   <c:userShapes r:id="rId1"/>
@@ -9037,7 +9033,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
     </c:title>
     <c:plotArea>
       <c:layout/>
@@ -9454,25 +9449,25 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="64686720"/>
-        <c:axId val="64696704"/>
+        <c:axId val="64620416"/>
+        <c:axId val="64621952"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="64686720"/>
+        <c:axId val="64620416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="64696704"/>
+        <c:crossAx val="64621952"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="64696704"/>
+        <c:axId val="64621952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9486,20 +9481,19 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="64686720"/>
+        <c:crossAx val="64620416"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -9918,11 +9912,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="64733568"/>
-        <c:axId val="64735488"/>
+        <c:axId val="64650240"/>
+        <c:axId val="64660608"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="64733568"/>
+        <c:axId val="64650240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9945,16 +9939,15 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="64735488"/>
+        <c:crossAx val="64660608"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="64735488"/>
+        <c:axId val="64660608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9977,11 +9970,10 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="64733568"/>
+        <c:crossAx val="64650240"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -9990,7 +9982,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
     <c:pageSetup/>
   </c:printSettings>
   <c:userShapes r:id="rId1"/>
@@ -10410,11 +10402,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="63341696"/>
-        <c:axId val="63343616"/>
+        <c:axId val="63534208"/>
+        <c:axId val="63536128"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="63341696"/>
+        <c:axId val="63534208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10441,12 +10433,12 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="63343616"/>
+        <c:crossAx val="63536128"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="63343616"/>
+        <c:axId val="63536128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10478,7 +10470,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="63341696"/>
+        <c:crossAx val="63534208"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -10487,7 +10479,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
+    <c:pageMargins b="0.75000000000000056" l="0.70000000000000051" r="0.70000000000000051" t="0.75000000000000056" header="0.30000000000000027" footer="0.30000000000000027"/>
     <c:pageSetup/>
   </c:printSettings>
   <c:userShapes r:id="rId1"/>
@@ -10931,25 +10923,25 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="64110592"/>
-        <c:axId val="64112128"/>
+        <c:axId val="63983616"/>
+        <c:axId val="63985152"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="64110592"/>
+        <c:axId val="63983616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="64112128"/>
+        <c:crossAx val="63985152"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="64112128"/>
+        <c:axId val="63985152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10963,7 +10955,7 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="64110592"/>
+        <c:crossAx val="63983616"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -10976,7 +10968,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
+    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -11396,11 +11388,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="64140416"/>
-        <c:axId val="64142336"/>
+        <c:axId val="64013440"/>
+        <c:axId val="64015360"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="64140416"/>
+        <c:axId val="64013440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11427,12 +11419,12 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="64142336"/>
+        <c:crossAx val="64015360"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="64142336"/>
+        <c:axId val="64015360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11463,7 +11455,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="64140416"/>
+        <c:crossAx val="64013440"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -11472,7 +11464,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
+    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
     <c:pageSetup/>
   </c:printSettings>
   <c:userShapes r:id="rId1"/>
@@ -11916,25 +11908,25 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="64155008"/>
-        <c:axId val="64222720"/>
+        <c:axId val="64065920"/>
+        <c:axId val="64148992"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="64155008"/>
+        <c:axId val="64065920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="64222720"/>
+        <c:crossAx val="64148992"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="64222720"/>
+        <c:axId val="64148992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11948,7 +11940,7 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="64155008"/>
+        <c:crossAx val="64065920"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -11961,7 +11953,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
+    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -12381,11 +12373,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="64160896"/>
-        <c:axId val="64162816"/>
+        <c:axId val="64111744"/>
+        <c:axId val="64113664"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="64160896"/>
+        <c:axId val="64111744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12412,12 +12404,12 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="64162816"/>
+        <c:crossAx val="64113664"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="64162816"/>
+        <c:axId val="64113664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12444,7 +12436,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="64160896"/>
+        <c:crossAx val="64111744"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -12453,7 +12445,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
+    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
     <c:pageSetup/>
   </c:printSettings>
   <c:userShapes r:id="rId1"/>
@@ -12897,25 +12889,25 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="64195968"/>
-        <c:axId val="64267392"/>
+        <c:axId val="64134528"/>
+        <c:axId val="64201856"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="64195968"/>
+        <c:axId val="64134528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="64267392"/>
+        <c:crossAx val="64201856"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="64267392"/>
+        <c:axId val="64201856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12929,7 +12921,7 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="64195968"/>
+        <c:crossAx val="64134528"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -12942,7 +12934,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
+    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -13361,11 +13353,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="64291584"/>
-        <c:axId val="64293504"/>
+        <c:axId val="64217856"/>
+        <c:axId val="64219776"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="64291584"/>
+        <c:axId val="64217856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13392,12 +13384,12 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="64293504"/>
+        <c:crossAx val="64219776"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="64293504"/>
+        <c:axId val="64219776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13424,7 +13416,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="64291584"/>
+        <c:crossAx val="64217856"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -13433,7 +13425,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
+    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
     <c:pageSetup/>
   </c:printSettings>
   <c:userShapes r:id="rId1"/>
@@ -13877,25 +13869,25 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="64351232"/>
-        <c:axId val="64361216"/>
+        <c:axId val="64285696"/>
+        <c:axId val="64295680"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="64351232"/>
+        <c:axId val="64285696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="64361216"/>
+        <c:crossAx val="64295680"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="64361216"/>
+        <c:axId val="64295680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13909,7 +13901,7 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="64351232"/>
+        <c:crossAx val="64285696"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -13922,7 +13914,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
+    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -14379,8 +14371,8 @@
       <xdr:rowOff>180974</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>552450</xdr:colOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>590550</xdr:colOff>
       <xdr:row>16</xdr:row>
       <xdr:rowOff>95249</xdr:rowOff>
     </xdr:to>
@@ -14582,8 +14574,8 @@
       <xdr:rowOff>104775</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>171450</xdr:colOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>581025</xdr:colOff>
       <xdr:row>14</xdr:row>
       <xdr:rowOff>180975</xdr:rowOff>
     </xdr:to>
@@ -14692,14 +14684,14 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>761999</xdr:colOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>7</xdr:row>
       <xdr:rowOff>66675</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>561974</xdr:colOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>619126</xdr:colOff>
       <xdr:row>21</xdr:row>
       <xdr:rowOff>142875</xdr:rowOff>
     </xdr:to>
@@ -14814,8 +14806,8 @@
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>400050</xdr:colOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>619125</xdr:colOff>
       <xdr:row>22</xdr:row>
       <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
@@ -15156,7 +15148,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:U63"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="Q30" sqref="Q30"/>
     </sheetView>
   </sheetViews>
@@ -16247,8 +16239,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:P63"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="P21" sqref="P21:P26"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -16975,8 +16967,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:O63"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="Q18" sqref="Q18"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="N31" sqref="N31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -17703,8 +17695,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E63"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F55" sqref="F55"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="P22" sqref="P22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -18430,8 +18422,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E63"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O35" sqref="O35"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="N26" sqref="N26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>

</xml_diff>